<commit_message>
system test approved by tl :)
</commit_message>
<xml_diff>
--- a/SimpCity US4 Test Document (3 Pass 0 Fail).xlsx
+++ b/SimpCity US4 Test Document (3 Pass 0 Fail).xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huiyi\Downloads\Year 3-Poly\Sem 3.2 DevOps\Tesr Documents\Sprint 4 V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EABBEDA-04F4-4A4A-88D2-B32FBE14FC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07669CE-B0BD-4DD5-BCB1-34A798F674F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US4 Sprint 4" sheetId="21" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="62">
   <si>
     <t>Test Scenarios for SimpCity</t>
   </si>
@@ -302,6 +302,9 @@
       </rPr>
       <t>: Option "2" is not implemented in Sprint 4</t>
     </r>
+  </si>
+  <si>
+    <t>claris</t>
   </si>
 </sst>
 </file>
@@ -1226,56 +1229,56 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1939,31 +1942,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85328E9-D433-4B7C-A93F-273BC750ECF2}">
   <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" customWidth="1"/>
+    <col min="5" max="5" width="44.5546875" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="18" style="67" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="123.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="123.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="124"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="38"/>
       <c r="E1" s="36"/>
       <c r="F1" s="40"/>
@@ -1974,29 +1977,29 @@
       <c r="K1" s="10"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="121"/>
+      <c r="C2" s="123"/>
       <c r="D2" s="13"/>
-      <c r="E2" s="120" t="s">
+      <c r="E2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="121"/>
+      <c r="F2" s="123"/>
       <c r="G2" s="83"/>
-      <c r="H2" s="121" t="s">
+      <c r="H2" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="121"/>
-      <c r="J2" s="120" t="s">
+      <c r="I2" s="123"/>
+      <c r="J2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="122"/>
+      <c r="K2" s="109"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="22" t="s">
         <v>5</v>
@@ -2026,7 +2029,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="45" t="s">
         <v>10</v>
@@ -2054,7 +2057,7 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="24" t="s">
         <v>16</v>
@@ -2082,7 +2085,7 @@
       </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="27" t="s">
         <v>17</v>
@@ -2110,26 +2113,26 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="123"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="123" t="s">
+      <c r="E7" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="123"/>
+      <c r="F7" s="118"/>
       <c r="G7" s="84"/>
-      <c r="H7" s="123" t="s">
+      <c r="H7" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="123"/>
+      <c r="I7" s="118"/>
       <c r="J7"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="58" t="s">
         <v>24</v>
@@ -2155,7 +2158,7 @@
       <c r="K8" s="34"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="46"/>
       <c r="C9" s="55"/>
@@ -2164,7 +2167,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="G9" s="84"/>
       <c r="H9" s="63" t="s">
@@ -2177,7 +2180,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
@@ -2193,7 +2196,7 @@
       <c r="K10" s="9"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -2207,7 +2210,7 @@
       <c r="K11" s="11"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="68"/>
       <c r="B12" s="12"/>
       <c r="C12" s="52"/>
@@ -2220,7 +2223,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
     </row>
-    <row r="13" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="69" t="s">
         <v>27</v>
       </c>
@@ -2255,31 +2258,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="66" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="109">
+    <row r="14" spans="1:12" s="66" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="110">
         <v>1</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="112" t="s">
+      <c r="C14" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="114" t="s">
+      <c r="D14" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="115"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="117"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="118"/>
-      <c r="K14" s="119"/>
-    </row>
-    <row r="15" spans="1:12" ht="319.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="109"/>
-      <c r="B15" s="111"/>
-      <c r="C15" s="113"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="121"/>
+    </row>
+    <row r="15" spans="1:12" ht="319.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="110"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="114"/>
       <c r="D15" s="81" t="s">
         <v>46</v>
       </c>
@@ -2301,7 +2304,7 @@
       </c>
       <c r="K15" s="79"/>
     </row>
-    <row r="16" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="95">
         <v>2</v>
       </c>
@@ -2317,7 +2320,7 @@
       <c r="E16" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="108" t="s">
+      <c r="F16" s="124" t="s">
         <v>41</v>
       </c>
       <c r="G16" s="93" t="s">
@@ -2334,7 +2337,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:41" s="77" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" s="77" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="94">
         <v>3</v>
       </c>
@@ -2350,7 +2353,7 @@
       <c r="E17" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="108"/>
+      <c r="F17" s="124"/>
       <c r="G17" s="89" t="s">
         <v>39</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:41" s="101" customFormat="1" ht="302.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" s="101" customFormat="1" ht="302.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="90"/>
       <c r="B18"/>
       <c r="C18" s="73"/>
@@ -2408,28 +2411,28 @@
       <c r="AN18"/>
       <c r="AO18" s="8"/>
     </row>
-    <row r="19" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
-      <c r="B19" s="120" t="s">
+      <c r="B19" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="121"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="120" t="s">
+      <c r="E19" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="121"/>
+      <c r="F19" s="123"/>
       <c r="G19" s="83"/>
-      <c r="H19" s="121" t="s">
+      <c r="H19" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="121"/>
-      <c r="J19" s="120" t="s">
+      <c r="I19" s="123"/>
+      <c r="J19" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="122"/>
-    </row>
-    <row r="20" spans="1:41" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="K19" s="109"/>
+    </row>
+    <row r="20" spans="1:41" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="22" t="s">
         <v>5</v>
@@ -2458,7 +2461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="45" t="s">
         <v>10</v>
@@ -2485,7 +2488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="24" t="s">
         <v>16</v>
@@ -2512,7 +2515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="27" t="s">
         <v>17</v>
@@ -2539,25 +2542,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="123" t="s">
+      <c r="B24" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="123"/>
+      <c r="C24" s="118"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="123" t="s">
+      <c r="E24" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="123"/>
+      <c r="F24" s="118"/>
       <c r="G24" s="84"/>
-      <c r="H24" s="123" t="s">
+      <c r="H24" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="123"/>
+      <c r="I24" s="118"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="58" t="s">
         <v>24</v>
@@ -2582,7 +2585,7 @@
       <c r="J25" s="43"/>
       <c r="K25" s="34"/>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="46"/>
       <c r="C26" s="55"/>
@@ -2603,7 +2606,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="D27" s="4"/>
       <c r="E27" s="1"/>
@@ -2618,7 +2621,7 @@
       <c r="J27" s="21"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -2631,7 +2634,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" s="68"/>
       <c r="B29" s="12"/>
       <c r="C29" s="52"/>
@@ -2644,7 +2647,7 @@
       <c r="J29" s="14"/>
       <c r="K29" s="15"/>
     </row>
-    <row r="30" spans="1:41" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A30" s="69" t="s">
         <v>27</v>
       </c>
@@ -2679,31 +2682,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A31" s="109">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A31" s="110">
         <v>1</v>
       </c>
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="112" t="s">
+      <c r="C31" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="114" t="s">
+      <c r="D31" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="115"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="117"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="118"/>
-      <c r="J31" s="118"/>
-      <c r="K31" s="119"/>
-    </row>
-    <row r="32" spans="1:41" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="109"/>
-      <c r="B32" s="111"/>
-      <c r="C32" s="113"/>
+      <c r="E31" s="116"/>
+      <c r="F31" s="117"/>
+      <c r="G31" s="119"/>
+      <c r="H31" s="120"/>
+      <c r="I31" s="120"/>
+      <c r="J31" s="120"/>
+      <c r="K31" s="121"/>
+    </row>
+    <row r="32" spans="1:41" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="110"/>
+      <c r="B32" s="112"/>
+      <c r="C32" s="114"/>
       <c r="D32" s="81" t="s">
         <v>46</v>
       </c>
@@ -2727,7 +2730,7 @@
       </c>
       <c r="K32" s="79"/>
     </row>
-    <row r="33" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="95">
         <v>2</v>
       </c>
@@ -2743,7 +2746,7 @@
       <c r="E33" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="108" t="s">
+      <c r="F33" s="124" t="s">
         <v>41</v>
       </c>
       <c r="G33" s="93" t="s">
@@ -2758,7 +2761,7 @@
       </c>
       <c r="K33" s="107"/>
     </row>
-    <row r="34" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="94">
         <v>3</v>
       </c>
@@ -2774,7 +2777,7 @@
       <c r="E34" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="108"/>
+      <c r="F34" s="124"/>
       <c r="G34" s="89" t="s">
         <v>39</v>
       </c>
@@ -2789,6 +2792,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F16:F17"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
@@ -2798,24 +2819,6 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="G14:K14"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:F31"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F15:F16 F18 F32:F33" xr:uid="{E119BFFA-0D14-49B1-A951-B0ECD7493FEA}">

</xml_diff>